<commit_message>
Cleaned up script, coordinates now no longer included
</commit_message>
<xml_diff>
--- a/HutInfoSAC.xlsx
+++ b/HutInfoSAC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab62753a27e4e959/Projekte/SAC Scraper/FindFreeHut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0505979A5BB0510E13B93D11595ED87656CDC48A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58B6F9C0-D9D2-49FB-A899-743A5DBD355F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_0505979A5BB0510E13B93D11595ED87656CDC48A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17CC4D0B-7284-4A25-953E-6DA1ADA1D3E5}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2055" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="449">
   <si>
     <t>Hut ID</t>
   </si>
@@ -971,18 +971,6 @@
   </si>
   <si>
     <t>https://www.alpsonline.org/reservation/calendar?hut_id=341&amp;selectDate=11.07.2027&amp;lang=en</t>
-  </si>
-  <si>
-    <t>ZZZ TEST Monbijouhütte, SAC GS</t>
-  </si>
-  <si>
-    <t>666</t>
-  </si>
-  <si>
-    <t>XXX.XXX / YYY.YYY</t>
-  </si>
-  <si>
-    <t>https://www.alpsonline.org/reservation/calendar?hut_id=346&amp;selectDate=11.07.2027&amp;lang=en</t>
   </si>
   <si>
     <t>Schalijochbiwak SAC, SAC Basel</t>
@@ -1454,6 +1442,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1741,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,7 +3089,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B80" t="s">
         <v>317</v>
@@ -3114,7 +3106,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B81" t="s">
         <v>321</v>
@@ -3131,7 +3123,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B82" t="s">
         <v>325</v>
@@ -3148,7 +3140,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="B83" t="s">
         <v>329</v>
@@ -3165,7 +3157,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B84" t="s">
         <v>333</v>
@@ -3182,7 +3174,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B85" t="s">
         <v>337</v>
@@ -3199,7 +3191,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B86" t="s">
         <v>341</v>
@@ -3216,7 +3208,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B87" t="s">
         <v>345</v>
@@ -3233,7 +3225,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="B88" t="s">
         <v>349</v>
@@ -3250,7 +3242,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="B89" t="s">
         <v>353</v>
@@ -3267,7 +3259,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B90" t="s">
         <v>357</v>
@@ -3284,7 +3276,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="B91" t="s">
         <v>361</v>
@@ -3301,7 +3293,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="B92" t="s">
         <v>365</v>
@@ -3318,7 +3310,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B93" t="s">
         <v>369</v>
@@ -3335,30 +3327,30 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="B94" t="s">
         <v>373</v>
       </c>
       <c r="C94" t="s">
+        <v>326</v>
+      </c>
+      <c r="D94" t="s">
         <v>374</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>375</v>
-      </c>
-      <c r="E94" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>417</v>
+        <v>444</v>
       </c>
       <c r="B95" t="s">
+        <v>376</v>
+      </c>
+      <c r="C95" t="s">
         <v>377</v>
-      </c>
-      <c r="C95" t="s">
-        <v>330</v>
       </c>
       <c r="D95" t="s">
         <v>378</v>
@@ -3369,7 +3361,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B96" t="s">
         <v>380</v>
@@ -3386,7 +3378,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="B97" t="s">
         <v>384</v>
@@ -3403,7 +3395,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>453</v>
+        <v>486</v>
       </c>
       <c r="B98" t="s">
         <v>388</v>
@@ -3420,7 +3412,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B99" t="s">
         <v>392</v>
@@ -3437,7 +3429,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>487</v>
+        <v>498</v>
       </c>
       <c r="B100" t="s">
         <v>396</v>
@@ -3454,7 +3446,7 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>498</v>
+        <v>514</v>
       </c>
       <c r="B101" t="s">
         <v>400</v>
@@ -3471,30 +3463,30 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B102" t="s">
         <v>404</v>
       </c>
       <c r="C102" t="s">
+        <v>98</v>
+      </c>
+      <c r="D102" t="s">
         <v>405</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" t="s">
         <v>406</v>
-      </c>
-      <c r="E102" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="B103" t="s">
+        <v>407</v>
+      </c>
+      <c r="C103" t="s">
         <v>408</v>
-      </c>
-      <c r="C103" t="s">
-        <v>98</v>
       </c>
       <c r="D103" t="s">
         <v>409</v>
@@ -3505,7 +3497,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B104" t="s">
         <v>411</v>
@@ -3522,7 +3514,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B105" t="s">
         <v>415</v>
@@ -3539,7 +3531,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>530</v>
+        <v>558</v>
       </c>
       <c r="B106" t="s">
         <v>419</v>
@@ -3556,7 +3548,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B107" t="s">
         <v>423</v>
@@ -3573,7 +3565,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="B108" t="s">
         <v>427</v>
@@ -3590,7 +3582,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B109" t="s">
         <v>431</v>
@@ -3607,30 +3599,30 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="B110" t="s">
         <v>435</v>
       </c>
       <c r="C110" t="s">
+        <v>250</v>
+      </c>
+      <c r="D110" t="s">
         <v>436</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>437</v>
-      </c>
-      <c r="E110" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>579</v>
+        <v>603</v>
       </c>
       <c r="B111" t="s">
+        <v>438</v>
+      </c>
+      <c r="C111" t="s">
         <v>439</v>
-      </c>
-      <c r="C111" t="s">
-        <v>250</v>
       </c>
       <c r="D111" t="s">
         <v>440</v>
@@ -3641,53 +3633,36 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>603</v>
+        <v>615</v>
       </c>
       <c r="B112" t="s">
         <v>442</v>
       </c>
       <c r="C112" t="s">
+        <v>58</v>
+      </c>
+      <c r="D112" t="s">
         <v>443</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>444</v>
-      </c>
-      <c r="E112" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>615</v>
+        <v>665</v>
       </c>
       <c r="B113" t="s">
+        <v>445</v>
+      </c>
+      <c r="C113" t="s">
         <v>446</v>
-      </c>
-      <c r="C113" t="s">
-        <v>58</v>
       </c>
       <c r="D113" t="s">
         <v>447</v>
       </c>
       <c r="E113" t="s">
         <v>448</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>665</v>
-      </c>
-      <c r="B114" t="s">
-        <v>449</v>
-      </c>
-      <c r="C114" t="s">
-        <v>450</v>
-      </c>
-      <c r="D114" t="s">
-        <v>451</v>
-      </c>
-      <c r="E114" t="s">
-        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>